<commit_message>
Adding Sheet2 on Lane file
</commit_message>
<xml_diff>
--- a/MP_Lanes.xlsx
+++ b/MP_Lanes.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MP_Integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAE2E8D-FA0D-49B5-8C27-0F0AFC1D83A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77712D66-8841-4F0F-A69D-5F535F174B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{A4CF0ABE-14FD-42BB-B8A3-EC2C5CB86E34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{A4CF0ABE-14FD-42BB-B8A3-EC2C5CB86E34}"/>
   </bookViews>
   <sheets>
     <sheet name="LaneLegs_MP" sheetId="1" r:id="rId1"/>
     <sheet name="Lanes_MP" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
-    <sheet name="ProductInLanes_MP" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
+    <sheet name="ProductInLanes_MP" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="311">
   <si>
     <t>CO2Emission</t>
   </si>
@@ -969,6 +970,9 @@
   </si>
   <si>
     <t>testing 123</t>
+  </si>
+  <si>
+    <t>version working on git hub by made sheet2</t>
   </si>
 </sst>
 </file>
@@ -1545,7 +1549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ACE8295-D0D5-4CA8-BFA3-14AFAB294A1C}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1565,6 +1569,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B5612E-13E7-4DA8-ADD2-BDA1277EB5B0}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF659CB-0E11-40F8-803E-CBE16EF82B48}">
   <dimension ref="A1:C286"/>
   <sheetViews>

</xml_diff>